<commit_message>
modificacion para primer desafio tp final
</commit_message>
<xml_diff>
--- a/tablas bd - My Pets.xlsx
+++ b/tablas bd - My Pets.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="77">
   <si>
     <t>Tablas app My Pets</t>
   </si>
@@ -37,13 +37,13 @@
     <t>Detalle</t>
   </si>
   <si>
-    <t>usuario</t>
+    <t>user</t>
   </si>
   <si>
     <t>Contiene todos los usuarios registrados sin discriminar roles dentro de la app</t>
   </si>
   <si>
-    <t>id_usuario</t>
+    <t>id_user</t>
   </si>
   <si>
     <t>INT</t>
@@ -61,205 +61,187 @@
     <t>VARCHAR (50)</t>
   </si>
   <si>
-    <t>UNIQUE</t>
+    <t>UNIQUE NOT NULL</t>
   </si>
   <si>
-    <t>contraseña</t>
+    <t>password</t>
   </si>
   <si>
     <t>NOT NULL</t>
   </si>
   <si>
-    <t>dueño</t>
+    <t>owner</t>
   </si>
   <si>
     <t>Tabla de dueños de mascotas, asociada a un usuario en particular</t>
   </si>
   <si>
-    <t>id_dueño</t>
+    <t>id_owner</t>
   </si>
   <si>
-    <t>nombre</t>
+    <t>id_user_owner</t>
+  </si>
+  <si>
+    <t>name</t>
   </si>
   <si>
     <t>VARCHAR (30)</t>
   </si>
   <si>
-    <t>apellido</t>
+    <t>last_name</t>
   </si>
   <si>
-    <t>telefono</t>
+    <t>phone</t>
   </si>
   <si>
     <t>VARCHAR (15)</t>
   </si>
   <si>
-    <t>direccion</t>
+    <t>address</t>
   </si>
   <si>
     <t>VARCHAR (100)</t>
   </si>
   <si>
-    <t>veterinario</t>
+    <t>vet</t>
   </si>
   <si>
     <t>Tabla de veterinarios, asociada a un usuario en particular</t>
   </si>
   <si>
-    <t>id_veterinario</t>
+    <t>id_vet</t>
   </si>
   <si>
-    <t>urgencia</t>
+    <t>id_user_vet</t>
   </si>
   <si>
-    <t>BOOLEAN</t>
+    <t>emergency</t>
   </si>
   <si>
-    <t>mascota</t>
+    <t>INT (BOOLEAN)</t>
+  </si>
+  <si>
+    <t>NOT NULL DEFAULT 0</t>
+  </si>
+  <si>
+    <t>pet</t>
   </si>
   <si>
     <t>Mascotas, asociadas obligatoriamente a un dueño.</t>
   </si>
   <si>
-    <t>id_mascota</t>
+    <t>id_pet</t>
   </si>
   <si>
-    <t>id_alimento</t>
+    <t>id_food</t>
   </si>
   <si>
-    <t>especie</t>
+    <t>species</t>
   </si>
   <si>
-    <t>descripción</t>
+    <t>description</t>
   </si>
   <si>
     <t>TEXT</t>
   </si>
   <si>
-    <t>fecha_de_nacimiento</t>
+    <t>birthday</t>
   </si>
   <si>
     <t>DATE</t>
   </si>
   <si>
-    <t>ficha_medica</t>
+    <t>breed</t>
+  </si>
+  <si>
+    <t>medical_history</t>
   </si>
   <si>
     <t>Ficha de informacion medica de cada mascota, puede relacionarse con atenciones y cirugias de manera opcional</t>
   </si>
   <si>
-    <t>id_ficha_medica</t>
+    <t>id_medical_history</t>
   </si>
   <si>
-    <t>peso</t>
+    <t>id_pet_medical_history</t>
+  </si>
+  <si>
+    <t>weight</t>
   </si>
   <si>
     <t>FLOAT</t>
   </si>
   <si>
-    <t>tratamientos</t>
+    <t>medical_summary</t>
   </si>
   <si>
-    <t>enfermedades_base</t>
-  </si>
-  <si>
-    <t>cantidad_alimento (Grs.)</t>
-  </si>
-  <si>
-    <t>suplementos</t>
-  </si>
-  <si>
-    <t>alimento</t>
-  </si>
-  <si>
-    <t>Tabla con marcas de alimentos y sus caracteristicas, cargada por admin,</t>
-  </si>
-  <si>
-    <t>marca</t>
-  </si>
-  <si>
-    <t>version</t>
-  </si>
-  <si>
-    <t>caracteristicas</t>
-  </si>
-  <si>
-    <t>atencion</t>
+    <t>appointment</t>
   </si>
   <si>
     <t>Tabla que contiene cada atencion que se le realiza a la mascota, se debe indicar obligatoriamente un veterinario y una historia clinica</t>
   </si>
   <si>
-    <t>id_atencion</t>
+    <t>id_appointment</t>
   </si>
   <si>
-    <t>id_historia_cliinica</t>
-  </si>
-  <si>
-    <t>fecha</t>
+    <t>date</t>
   </si>
   <si>
     <t>DATETIME</t>
   </si>
   <si>
-    <t>diagnostico_ingreso</t>
+    <t>diagnosis</t>
   </si>
   <si>
-    <t>cirugia</t>
+    <t>surgery</t>
   </si>
   <si>
     <t>Tabla que contiene cada cirugia que se le realiza a la mascota, se debe indicar obligatoriamente un veterinario y una historia clinica</t>
   </si>
   <si>
-    <t>id_cirugia</t>
+    <t>id_surgery</t>
   </si>
   <si>
-    <t>tratamiento</t>
+    <t>treatment</t>
   </si>
   <si>
     <t>Tabla que contiene cada tratamiento propuesto que se le realiza a la mascota dentro de una atencion, por ejemplo, dentro de una atencion, se puede indicar una sutura de herida y un inyectable, siendo tratamientos distintos dentro de una misma atencion.</t>
   </si>
   <si>
-    <t>id_tratamiento</t>
+    <t>id_treatment</t>
   </si>
   <si>
-    <t>medicamento</t>
+    <t>medicine</t>
   </si>
   <si>
-    <t>duración</t>
+    <t>end_date</t>
   </si>
   <si>
-    <t>descripcion</t>
-  </si>
-  <si>
-    <t>tratamiento_medicamento</t>
+    <t>treatment_medicine</t>
   </si>
   <si>
     <t>Tabla intermedia</t>
   </si>
   <si>
-    <t>id_tratamiento_medicamento</t>
+    <t>id_treatment_medicine</t>
   </si>
   <si>
-    <t>id_medicamento</t>
+    <t>id_medicine</t>
   </si>
   <si>
     <t>Tabla con medicamentos y sus caracteristicas, cargada por admin</t>
   </si>
   <si>
-    <t>droga</t>
+    <t>drug</t>
   </si>
   <si>
-    <t>tipo_administracion</t>
+    <t>administration</t>
   </si>
   <si>
-    <t>ENUM</t>
+    <t>type</t>
   </si>
   <si>
-    <t>tipo</t>
-  </si>
-  <si>
-    <t>colocacion_periodica</t>
+    <t>periodic</t>
   </si>
 </sst>
 </file>
@@ -567,7 +549,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="68">
+  <cellXfs count="66">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -719,9 +701,6 @@
     <xf borderId="11" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="12" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf borderId="14" fillId="2" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" vertical="center"/>
     </xf>
@@ -732,23 +711,20 @@
       <alignment horizontal="left" readingOrder="0" vertical="center"/>
     </xf>
     <xf borderId="12" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf borderId="12" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" vertical="center"/>
     </xf>
     <xf borderId="16" fillId="0" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="17" fillId="0" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="18" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="18" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" vertical="center"/>
     </xf>
-    <xf borderId="18" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="18" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" vertical="center"/>
     </xf>
-    <xf borderId="18" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="18" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="19" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="19" fillId="2" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" vertical="center"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -991,10 +967,10 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="25.5"/>
-    <col customWidth="1" min="2" max="2" width="23.25"/>
-    <col customWidth="1" min="3" max="3" width="24.5"/>
-    <col customWidth="1" min="4" max="4" width="18.0"/>
+    <col customWidth="1" min="1" max="1" width="19.0"/>
+    <col customWidth="1" min="2" max="2" width="28.88"/>
+    <col customWidth="1" min="3" max="3" width="25.25"/>
+    <col customWidth="1" min="4" max="4" width="16.0"/>
     <col customWidth="1" min="5" max="6" width="4.5"/>
     <col customWidth="1" min="7" max="7" width="24.75"/>
   </cols>
@@ -1118,7 +1094,7 @@
       <c r="A8" s="19"/>
       <c r="B8" s="20"/>
       <c r="C8" s="33" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="D8" s="34" t="s">
         <v>11</v>
@@ -1135,10 +1111,10 @@
       <c r="A9" s="19"/>
       <c r="B9" s="20"/>
       <c r="C9" s="33" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D9" s="34" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E9" s="31"/>
       <c r="F9" s="31"/>
@@ -1150,10 +1126,10 @@
       <c r="A10" s="19"/>
       <c r="B10" s="20"/>
       <c r="C10" s="33" t="s">
+        <v>25</v>
+      </c>
+      <c r="D10" s="34" t="s">
         <v>24</v>
-      </c>
-      <c r="D10" s="34" t="s">
-        <v>23</v>
       </c>
       <c r="E10" s="31"/>
       <c r="F10" s="31"/>
@@ -1165,10 +1141,10 @@
       <c r="A11" s="19"/>
       <c r="B11" s="20"/>
       <c r="C11" s="33" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D11" s="36" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E11" s="31"/>
       <c r="F11" s="31"/>
@@ -1180,10 +1156,10 @@
       <c r="A12" s="25"/>
       <c r="B12" s="26"/>
       <c r="C12" s="33" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D12" s="34" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E12" s="31"/>
       <c r="F12" s="31"/>
@@ -1193,13 +1169,13 @@
     </row>
     <row r="13">
       <c r="A13" s="37" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B13" s="38" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C13" s="39" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D13" s="40" t="s">
         <v>11</v>
@@ -1216,7 +1192,7 @@
       <c r="A14" s="19"/>
       <c r="B14" s="20"/>
       <c r="C14" s="21" t="s">
-        <v>10</v>
+        <v>33</v>
       </c>
       <c r="D14" s="22" t="s">
         <v>11</v>
@@ -1233,10 +1209,10 @@
       <c r="A15" s="19"/>
       <c r="B15" s="20"/>
       <c r="C15" s="21" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D15" s="22" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E15" s="23"/>
       <c r="F15" s="23"/>
@@ -1248,10 +1224,10 @@
       <c r="A16" s="19"/>
       <c r="B16" s="20"/>
       <c r="C16" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="D16" s="22" t="s">
         <v>24</v>
-      </c>
-      <c r="D16" s="22" t="s">
-        <v>23</v>
       </c>
       <c r="E16" s="23"/>
       <c r="F16" s="23"/>
@@ -1263,10 +1239,10 @@
       <c r="A17" s="19"/>
       <c r="B17" s="20"/>
       <c r="C17" s="21" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D17" s="42" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E17" s="23"/>
       <c r="F17" s="23"/>
@@ -1278,10 +1254,10 @@
       <c r="A18" s="19"/>
       <c r="B18" s="20"/>
       <c r="C18" s="21" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D18" s="22" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E18" s="23"/>
       <c r="F18" s="23"/>
@@ -1293,26 +1269,26 @@
       <c r="A19" s="25"/>
       <c r="B19" s="26"/>
       <c r="C19" s="21" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D19" s="22" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="E19" s="23"/>
       <c r="F19" s="23"/>
       <c r="G19" s="24" t="s">
-        <v>18</v>
+        <v>36</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="27" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="B20" s="28" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="C20" s="29" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="D20" s="30" t="s">
         <v>11</v>
@@ -1346,7 +1322,7 @@
       <c r="A22" s="19"/>
       <c r="B22" s="20"/>
       <c r="C22" s="33" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="D22" s="34" t="s">
         <v>11</v>
@@ -1361,10 +1337,10 @@
       <c r="A23" s="19"/>
       <c r="B23" s="20"/>
       <c r="C23" s="33" t="s">
-        <v>38</v>
+        <v>23</v>
       </c>
       <c r="D23" s="34" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E23" s="31"/>
       <c r="F23" s="31"/>
@@ -1376,10 +1352,10 @@
       <c r="A24" s="19"/>
       <c r="B24" s="20"/>
       <c r="C24" s="33" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D24" s="34" t="s">
-        <v>40</v>
+        <v>24</v>
       </c>
       <c r="E24" s="31"/>
       <c r="F24" s="31"/>
@@ -1390,26 +1366,26 @@
     <row r="25">
       <c r="A25" s="19"/>
       <c r="B25" s="20"/>
-      <c r="C25" s="45" t="s">
-        <v>41</v>
-      </c>
-      <c r="D25" s="46" t="s">
+      <c r="C25" s="33" t="s">
         <v>42</v>
       </c>
-      <c r="E25" s="47"/>
-      <c r="F25" s="47"/>
+      <c r="D25" s="34" t="s">
+        <v>43</v>
+      </c>
+      <c r="E25" s="31"/>
+      <c r="F25" s="31"/>
       <c r="G25" s="35" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="26">
-      <c r="A26" s="25"/>
-      <c r="B26" s="26"/>
+      <c r="A26" s="19"/>
+      <c r="B26" s="20"/>
       <c r="C26" s="45" t="s">
-        <v>27</v>
-      </c>
-      <c r="D26" s="34" t="s">
-        <v>28</v>
+        <v>44</v>
+      </c>
+      <c r="D26" s="46" t="s">
+        <v>45</v>
       </c>
       <c r="E26" s="47"/>
       <c r="F26" s="47"/>
@@ -1418,55 +1394,55 @@
       </c>
     </row>
     <row r="27">
-      <c r="A27" s="48" t="s">
-        <v>43</v>
-      </c>
-      <c r="B27" s="49" t="s">
-        <v>44</v>
-      </c>
-      <c r="C27" s="50" t="s">
-        <v>45</v>
-      </c>
-      <c r="D27" s="40" t="s">
+      <c r="A27" s="25"/>
+      <c r="B27" s="26"/>
+      <c r="C27" s="45" t="s">
+        <v>46</v>
+      </c>
+      <c r="D27" s="34" t="s">
+        <v>29</v>
+      </c>
+      <c r="E27" s="47"/>
+      <c r="F27" s="47"/>
+      <c r="G27" s="35" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="48" t="s">
+        <v>47</v>
+      </c>
+      <c r="B28" s="49" t="s">
+        <v>48</v>
+      </c>
+      <c r="C28" s="50" t="s">
+        <v>49</v>
+      </c>
+      <c r="D28" s="40" t="s">
         <v>11</v>
       </c>
-      <c r="E27" s="40" t="s">
+      <c r="E28" s="40" t="s">
         <v>12</v>
       </c>
-      <c r="F27" s="23"/>
-      <c r="G27" s="41" t="s">
+      <c r="F28" s="23"/>
+      <c r="G28" s="41" t="s">
         <v>13</v>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" s="19"/>
-      <c r="B28" s="20"/>
-      <c r="C28" s="51" t="s">
-        <v>36</v>
-      </c>
-      <c r="D28" s="22" t="s">
-        <v>11</v>
-      </c>
-      <c r="E28" s="23"/>
-      <c r="F28" s="40" t="s">
-        <v>12</v>
-      </c>
-      <c r="G28" s="52" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="19"/>
       <c r="B29" s="20"/>
       <c r="C29" s="51" t="s">
-        <v>46</v>
-      </c>
-      <c r="D29" s="53" t="s">
-        <v>47</v>
-      </c>
-      <c r="E29" s="54"/>
-      <c r="F29" s="54"/>
-      <c r="G29" s="24" t="s">
+        <v>50</v>
+      </c>
+      <c r="D29" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="E29" s="23"/>
+      <c r="F29" s="40" t="s">
+        <v>12</v>
+      </c>
+      <c r="G29" s="52" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1474,85 +1450,95 @@
       <c r="A30" s="19"/>
       <c r="B30" s="20"/>
       <c r="C30" s="51" t="s">
-        <v>48</v>
-      </c>
-      <c r="D30" s="22" t="s">
-        <v>15</v>
+        <v>51</v>
+      </c>
+      <c r="D30" s="53" t="s">
+        <v>52</v>
       </c>
       <c r="E30" s="54"/>
       <c r="F30" s="54"/>
-      <c r="G30" s="55"/>
+      <c r="G30" s="24" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="31">
-      <c r="A31" s="19"/>
-      <c r="B31" s="20"/>
+      <c r="A31" s="25"/>
+      <c r="B31" s="26"/>
       <c r="C31" s="51" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="D31" s="22" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E31" s="54"/>
       <c r="F31" s="54"/>
-      <c r="G31" s="55"/>
+      <c r="G31" s="52" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="32">
-      <c r="A32" s="19"/>
-      <c r="B32" s="20"/>
-      <c r="C32" s="51" t="s">
-        <v>50</v>
-      </c>
-      <c r="D32" s="53" t="s">
+      <c r="A32" s="55" t="s">
+        <v>54</v>
+      </c>
+      <c r="B32" s="56" t="s">
+        <v>55</v>
+      </c>
+      <c r="C32" s="57" t="s">
+        <v>56</v>
+      </c>
+      <c r="D32" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="E32" s="54"/>
-      <c r="F32" s="54"/>
-      <c r="G32" s="24" t="s">
+      <c r="E32" s="30" t="s">
+        <v>12</v>
+      </c>
+      <c r="F32" s="31"/>
+      <c r="G32" s="32" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="19"/>
+      <c r="B33" s="20"/>
+      <c r="C33" s="45" t="s">
+        <v>32</v>
+      </c>
+      <c r="D33" s="34" t="s">
+        <v>11</v>
+      </c>
+      <c r="E33" s="31"/>
+      <c r="F33" s="30" t="s">
+        <v>12</v>
+      </c>
+      <c r="G33" s="58" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="33">
-      <c r="A33" s="25"/>
-      <c r="B33" s="26"/>
-      <c r="C33" s="51" t="s">
-        <v>51</v>
-      </c>
-      <c r="D33" s="22" t="s">
-        <v>28</v>
-      </c>
-      <c r="E33" s="54"/>
-      <c r="F33" s="54"/>
-      <c r="G33" s="55"/>
-    </row>
     <row r="34">
-      <c r="A34" s="56" t="s">
-        <v>52</v>
-      </c>
-      <c r="B34" s="57" t="s">
-        <v>53</v>
-      </c>
-      <c r="C34" s="58" t="s">
-        <v>37</v>
-      </c>
-      <c r="D34" s="30" t="s">
+      <c r="A34" s="19"/>
+      <c r="B34" s="20"/>
+      <c r="C34" s="45" t="s">
+        <v>49</v>
+      </c>
+      <c r="D34" s="34" t="s">
         <v>11</v>
       </c>
-      <c r="E34" s="30" t="s">
+      <c r="E34" s="31"/>
+      <c r="F34" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="F34" s="31"/>
-      <c r="G34" s="32" t="s">
-        <v>13</v>
+      <c r="G34" s="58" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="19"/>
       <c r="B35" s="20"/>
       <c r="C35" s="45" t="s">
-        <v>54</v>
-      </c>
-      <c r="D35" s="34" t="s">
-        <v>15</v>
+        <v>57</v>
+      </c>
+      <c r="D35" s="46" t="s">
+        <v>58</v>
       </c>
       <c r="E35" s="47"/>
       <c r="F35" s="47"/>
@@ -1561,57 +1547,63 @@
       </c>
     </row>
     <row r="36">
-      <c r="A36" s="19"/>
-      <c r="B36" s="20"/>
+      <c r="A36" s="25"/>
+      <c r="B36" s="26"/>
       <c r="C36" s="45" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="D36" s="34" t="s">
-        <v>15</v>
+        <v>43</v>
       </c>
       <c r="E36" s="47"/>
       <c r="F36" s="47"/>
-      <c r="G36" s="59"/>
+      <c r="G36" s="35" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="37">
-      <c r="A37" s="25"/>
-      <c r="B37" s="26"/>
-      <c r="C37" s="45" t="s">
-        <v>56</v>
-      </c>
-      <c r="D37" s="34" t="s">
-        <v>40</v>
-      </c>
-      <c r="E37" s="47"/>
-      <c r="F37" s="47"/>
-      <c r="G37" s="59"/>
+      <c r="A37" s="48" t="s">
+        <v>60</v>
+      </c>
+      <c r="B37" s="49" t="s">
+        <v>61</v>
+      </c>
+      <c r="C37" s="50" t="s">
+        <v>62</v>
+      </c>
+      <c r="D37" s="40" t="s">
+        <v>11</v>
+      </c>
+      <c r="E37" s="40" t="s">
+        <v>12</v>
+      </c>
+      <c r="F37" s="23"/>
+      <c r="G37" s="41" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="38">
-      <c r="A38" s="48" t="s">
-        <v>57</v>
-      </c>
-      <c r="B38" s="49" t="s">
-        <v>58</v>
-      </c>
-      <c r="C38" s="50" t="s">
-        <v>59</v>
-      </c>
-      <c r="D38" s="40" t="s">
+      <c r="A38" s="19"/>
+      <c r="B38" s="20"/>
+      <c r="C38" s="51" t="s">
+        <v>32</v>
+      </c>
+      <c r="D38" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="E38" s="40" t="s">
+      <c r="E38" s="23"/>
+      <c r="F38" s="40" t="s">
         <v>12</v>
       </c>
-      <c r="F38" s="23"/>
-      <c r="G38" s="41" t="s">
-        <v>13</v>
+      <c r="G38" s="52" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="19"/>
       <c r="B39" s="20"/>
       <c r="C39" s="51" t="s">
-        <v>31</v>
+        <v>49</v>
       </c>
       <c r="D39" s="22" t="s">
         <v>11</v>
@@ -1628,27 +1620,25 @@
       <c r="A40" s="19"/>
       <c r="B40" s="20"/>
       <c r="C40" s="51" t="s">
-        <v>60</v>
-      </c>
-      <c r="D40" s="22" t="s">
-        <v>11</v>
-      </c>
-      <c r="E40" s="23"/>
-      <c r="F40" s="40" t="s">
-        <v>12</v>
-      </c>
-      <c r="G40" s="52" t="s">
+        <v>57</v>
+      </c>
+      <c r="D40" s="53" t="s">
+        <v>58</v>
+      </c>
+      <c r="E40" s="54"/>
+      <c r="F40" s="54"/>
+      <c r="G40" s="24" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="41">
-      <c r="A41" s="19"/>
-      <c r="B41" s="20"/>
+      <c r="A41" s="25"/>
+      <c r="B41" s="26"/>
       <c r="C41" s="51" t="s">
-        <v>61</v>
-      </c>
-      <c r="D41" s="53" t="s">
-        <v>62</v>
+        <v>59</v>
+      </c>
+      <c r="D41" s="22" t="s">
+        <v>43</v>
       </c>
       <c r="E41" s="54"/>
       <c r="F41" s="54"/>
@@ -1657,55 +1647,55 @@
       </c>
     </row>
     <row r="42">
-      <c r="A42" s="25"/>
-      <c r="B42" s="26"/>
-      <c r="C42" s="51" t="s">
+      <c r="A42" s="55" t="s">
         <v>63</v>
       </c>
-      <c r="D42" s="22" t="s">
-        <v>40</v>
-      </c>
-      <c r="E42" s="54"/>
-      <c r="F42" s="54"/>
-      <c r="G42" s="24" t="s">
+      <c r="B42" s="56" t="s">
+        <v>64</v>
+      </c>
+      <c r="C42" s="57" t="s">
+        <v>65</v>
+      </c>
+      <c r="D42" s="30" t="s">
+        <v>11</v>
+      </c>
+      <c r="E42" s="30" t="s">
+        <v>12</v>
+      </c>
+      <c r="F42" s="31"/>
+      <c r="G42" s="32" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="19"/>
+      <c r="B43" s="20"/>
+      <c r="C43" s="45" t="s">
+        <v>56</v>
+      </c>
+      <c r="D43" s="34" t="s">
+        <v>11</v>
+      </c>
+      <c r="E43" s="31"/>
+      <c r="F43" s="30" t="s">
+        <v>12</v>
+      </c>
+      <c r="G43" s="58" t="s">
         <v>18</v>
-      </c>
-    </row>
-    <row r="43">
-      <c r="A43" s="56" t="s">
-        <v>64</v>
-      </c>
-      <c r="B43" s="57" t="s">
-        <v>65</v>
-      </c>
-      <c r="C43" s="58" t="s">
-        <v>66</v>
-      </c>
-      <c r="D43" s="30" t="s">
-        <v>11</v>
-      </c>
-      <c r="E43" s="30" t="s">
-        <v>12</v>
-      </c>
-      <c r="F43" s="31"/>
-      <c r="G43" s="32" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="19"/>
       <c r="B44" s="20"/>
       <c r="C44" s="45" t="s">
-        <v>31</v>
-      </c>
-      <c r="D44" s="34" t="s">
-        <v>11</v>
-      </c>
-      <c r="E44" s="31"/>
-      <c r="F44" s="30" t="s">
-        <v>12</v>
-      </c>
-      <c r="G44" s="60" t="s">
+        <v>57</v>
+      </c>
+      <c r="D44" s="46" t="s">
+        <v>58</v>
+      </c>
+      <c r="E44" s="47"/>
+      <c r="F44" s="47"/>
+      <c r="G44" s="35" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1713,16 +1703,14 @@
       <c r="A45" s="19"/>
       <c r="B45" s="20"/>
       <c r="C45" s="45" t="s">
-        <v>60</v>
+        <v>23</v>
       </c>
       <c r="D45" s="34" t="s">
-        <v>11</v>
-      </c>
-      <c r="E45" s="31"/>
-      <c r="F45" s="30" t="s">
-        <v>12</v>
-      </c>
-      <c r="G45" s="60" t="s">
+        <v>15</v>
+      </c>
+      <c r="E45" s="47"/>
+      <c r="F45" s="47"/>
+      <c r="G45" s="35" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1730,10 +1718,10 @@
       <c r="A46" s="19"/>
       <c r="B46" s="20"/>
       <c r="C46" s="45" t="s">
-        <v>61</v>
-      </c>
-      <c r="D46" s="46" t="s">
-        <v>62</v>
+        <v>66</v>
+      </c>
+      <c r="D46" s="34" t="s">
+        <v>15</v>
       </c>
       <c r="E46" s="47"/>
       <c r="F46" s="47"/>
@@ -1742,13 +1730,13 @@
       </c>
     </row>
     <row r="47">
-      <c r="A47" s="25"/>
-      <c r="B47" s="26"/>
+      <c r="A47" s="19"/>
+      <c r="B47" s="20"/>
       <c r="C47" s="45" t="s">
-        <v>63</v>
-      </c>
-      <c r="D47" s="34" t="s">
-        <v>28</v>
+        <v>67</v>
+      </c>
+      <c r="D47" s="46" t="s">
+        <v>58</v>
       </c>
       <c r="E47" s="47"/>
       <c r="F47" s="47"/>
@@ -1757,272 +1745,228 @@
       </c>
     </row>
     <row r="48">
-      <c r="A48" s="48" t="s">
-        <v>67</v>
-      </c>
-      <c r="B48" s="49" t="s">
+      <c r="A48" s="25"/>
+      <c r="B48" s="26"/>
+      <c r="C48" s="45" t="s">
+        <v>42</v>
+      </c>
+      <c r="D48" s="34" t="s">
+        <v>43</v>
+      </c>
+      <c r="E48" s="47"/>
+      <c r="F48" s="47"/>
+      <c r="G48" s="35" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="48" t="s">
         <v>68</v>
       </c>
-      <c r="C48" s="50" t="s">
+      <c r="B49" s="49" t="s">
         <v>69</v>
       </c>
-      <c r="D48" s="40" t="s">
+      <c r="C49" s="50" t="s">
+        <v>70</v>
+      </c>
+      <c r="D49" s="40" t="s">
         <v>11</v>
       </c>
-      <c r="E48" s="40" t="s">
+      <c r="E49" s="40" t="s">
         <v>12</v>
       </c>
-      <c r="F48" s="23"/>
-      <c r="G48" s="41" t="s">
+      <c r="F49" s="23"/>
+      <c r="G49" s="41" t="s">
         <v>13</v>
-      </c>
-    </row>
-    <row r="49">
-      <c r="A49" s="19"/>
-      <c r="B49" s="20"/>
-      <c r="C49" s="51" t="s">
-        <v>59</v>
-      </c>
-      <c r="D49" s="22" t="s">
-        <v>11</v>
-      </c>
-      <c r="E49" s="23"/>
-      <c r="F49" s="40" t="s">
-        <v>12</v>
-      </c>
-      <c r="G49" s="52" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="19"/>
       <c r="B50" s="20"/>
       <c r="C50" s="51" t="s">
-        <v>61</v>
-      </c>
-      <c r="D50" s="53" t="s">
-        <v>62</v>
-      </c>
-      <c r="E50" s="54"/>
-      <c r="F50" s="54"/>
-      <c r="G50" s="24" t="s">
+        <v>71</v>
+      </c>
+      <c r="D50" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="E50" s="23"/>
+      <c r="F50" s="40" t="s">
+        <v>12</v>
+      </c>
+      <c r="G50" s="52" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="51">
-      <c r="A51" s="19"/>
-      <c r="B51" s="20"/>
+      <c r="A51" s="25"/>
+      <c r="B51" s="26"/>
       <c r="C51" s="51" t="s">
-        <v>22</v>
+        <v>65</v>
       </c>
       <c r="D51" s="22" t="s">
-        <v>15</v>
-      </c>
-      <c r="E51" s="54"/>
-      <c r="F51" s="54"/>
-      <c r="G51" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="E51" s="23"/>
+      <c r="F51" s="40" t="s">
+        <v>12</v>
+      </c>
+      <c r="G51" s="52" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="52">
-      <c r="A52" s="19"/>
-      <c r="B52" s="20"/>
-      <c r="C52" s="51" t="s">
-        <v>70</v>
-      </c>
-      <c r="D52" s="22" t="s">
-        <v>15</v>
-      </c>
-      <c r="E52" s="54"/>
-      <c r="F52" s="54"/>
-      <c r="G52" s="24" t="s">
-        <v>18</v>
+      <c r="A52" s="55" t="s">
+        <v>66</v>
+      </c>
+      <c r="B52" s="56" t="s">
+        <v>72</v>
+      </c>
+      <c r="C52" s="57" t="s">
+        <v>71</v>
+      </c>
+      <c r="D52" s="30" t="s">
+        <v>11</v>
+      </c>
+      <c r="E52" s="30" t="s">
+        <v>12</v>
+      </c>
+      <c r="F52" s="31"/>
+      <c r="G52" s="32" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="19"/>
       <c r="B53" s="20"/>
-      <c r="C53" s="51" t="s">
-        <v>71</v>
-      </c>
-      <c r="D53" s="53" t="s">
-        <v>62</v>
-      </c>
-      <c r="E53" s="54"/>
-      <c r="F53" s="54"/>
-      <c r="G53" s="24" t="s">
+      <c r="C53" s="45" t="s">
+        <v>23</v>
+      </c>
+      <c r="D53" s="34" t="s">
+        <v>24</v>
+      </c>
+      <c r="E53" s="47"/>
+      <c r="F53" s="47"/>
+      <c r="G53" s="35" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="54">
-      <c r="A54" s="25"/>
-      <c r="B54" s="26"/>
-      <c r="C54" s="51" t="s">
-        <v>72</v>
-      </c>
-      <c r="D54" s="22" t="s">
-        <v>40</v>
-      </c>
-      <c r="E54" s="54"/>
-      <c r="F54" s="54"/>
-      <c r="G54" s="24" t="s">
+      <c r="A54" s="19"/>
+      <c r="B54" s="20"/>
+      <c r="C54" s="45" t="s">
+        <v>73</v>
+      </c>
+      <c r="D54" s="34" t="s">
+        <v>15</v>
+      </c>
+      <c r="E54" s="47"/>
+      <c r="F54" s="47"/>
+      <c r="G54" s="35" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="55">
-      <c r="A55" s="56" t="s">
-        <v>73</v>
-      </c>
-      <c r="B55" s="57" t="s">
+      <c r="A55" s="19"/>
+      <c r="B55" s="20"/>
+      <c r="C55" s="45" t="s">
         <v>74</v>
       </c>
-      <c r="C55" s="58" t="s">
-        <v>75</v>
-      </c>
-      <c r="D55" s="30" t="s">
-        <v>11</v>
-      </c>
-      <c r="E55" s="30" t="s">
-        <v>12</v>
-      </c>
-      <c r="F55" s="31"/>
-      <c r="G55" s="32" t="s">
-        <v>13</v>
+      <c r="D55" s="34" t="s">
+        <v>24</v>
+      </c>
+      <c r="E55" s="47"/>
+      <c r="F55" s="47"/>
+      <c r="G55" s="35" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" s="19"/>
       <c r="B56" s="20"/>
       <c r="C56" s="45" t="s">
+        <v>75</v>
+      </c>
+      <c r="D56" s="34" t="s">
+        <v>24</v>
+      </c>
+      <c r="E56" s="47"/>
+      <c r="F56" s="47"/>
+      <c r="G56" s="35" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" s="59"/>
+      <c r="B57" s="60"/>
+      <c r="C57" s="61" t="s">
         <v>76</v>
       </c>
-      <c r="D56" s="34" t="s">
-        <v>11</v>
-      </c>
-      <c r="E56" s="31"/>
-      <c r="F56" s="30" t="s">
-        <v>12</v>
-      </c>
-      <c r="G56" s="60" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="57">
-      <c r="A57" s="25"/>
-      <c r="B57" s="26"/>
-      <c r="C57" s="45" t="s">
-        <v>69</v>
-      </c>
-      <c r="D57" s="34" t="s">
-        <v>11</v>
-      </c>
-      <c r="E57" s="31"/>
-      <c r="F57" s="30" t="s">
-        <v>12</v>
-      </c>
-      <c r="G57" s="60" t="s">
-        <v>18</v>
+      <c r="D57" s="62" t="s">
+        <v>35</v>
+      </c>
+      <c r="E57" s="63"/>
+      <c r="F57" s="63"/>
+      <c r="G57" s="64" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="58">
-      <c r="A58" s="48" t="s">
-        <v>70</v>
-      </c>
-      <c r="B58" s="49" t="s">
-        <v>77</v>
-      </c>
-      <c r="C58" s="50" t="s">
-        <v>76</v>
-      </c>
-      <c r="D58" s="40" t="s">
-        <v>11</v>
-      </c>
-      <c r="E58" s="40" t="s">
-        <v>12</v>
-      </c>
-      <c r="F58" s="23"/>
-      <c r="G58" s="41" t="s">
-        <v>13</v>
-      </c>
+      <c r="A58" s="1"/>
+      <c r="B58" s="65"/>
+      <c r="C58" s="3"/>
+      <c r="D58" s="1"/>
+      <c r="E58" s="4"/>
+      <c r="F58" s="4"/>
+      <c r="G58" s="1"/>
     </row>
     <row r="59">
-      <c r="A59" s="19"/>
-      <c r="B59" s="20"/>
-      <c r="C59" s="51" t="s">
-        <v>22</v>
-      </c>
-      <c r="D59" s="22" t="s">
-        <v>23</v>
-      </c>
-      <c r="E59" s="54"/>
-      <c r="F59" s="54"/>
-      <c r="G59" s="24" t="s">
-        <v>18</v>
-      </c>
+      <c r="A59" s="1"/>
+      <c r="B59" s="65"/>
+      <c r="C59" s="3"/>
+      <c r="D59" s="1"/>
+      <c r="E59" s="4"/>
+      <c r="F59" s="4"/>
+      <c r="G59" s="1"/>
     </row>
     <row r="60">
-      <c r="A60" s="19"/>
-      <c r="B60" s="20"/>
-      <c r="C60" s="51" t="s">
-        <v>78</v>
-      </c>
-      <c r="D60" s="22" t="s">
-        <v>15</v>
-      </c>
-      <c r="E60" s="54"/>
-      <c r="F60" s="54"/>
-      <c r="G60" s="24" t="s">
-        <v>18</v>
-      </c>
+      <c r="A60" s="1"/>
+      <c r="B60" s="65"/>
+      <c r="C60" s="3"/>
+      <c r="D60" s="1"/>
+      <c r="E60" s="4"/>
+      <c r="F60" s="4"/>
+      <c r="G60" s="1"/>
     </row>
     <row r="61">
-      <c r="A61" s="19"/>
-      <c r="B61" s="20"/>
-      <c r="C61" s="51" t="s">
-        <v>79</v>
-      </c>
-      <c r="D61" s="53" t="s">
-        <v>80</v>
-      </c>
-      <c r="E61" s="54"/>
-      <c r="F61" s="54"/>
-      <c r="G61" s="24" t="s">
-        <v>18</v>
-      </c>
+      <c r="A61" s="1"/>
+      <c r="B61" s="65"/>
+      <c r="C61" s="3"/>
+      <c r="D61" s="1"/>
+      <c r="E61" s="4"/>
+      <c r="F61" s="4"/>
+      <c r="G61" s="1"/>
     </row>
     <row r="62">
-      <c r="A62" s="19"/>
-      <c r="B62" s="20"/>
-      <c r="C62" s="51" t="s">
-        <v>81</v>
-      </c>
-      <c r="D62" s="53" t="s">
-        <v>80</v>
-      </c>
-      <c r="E62" s="54"/>
-      <c r="F62" s="54"/>
-      <c r="G62" s="24" t="s">
-        <v>18</v>
-      </c>
+      <c r="A62" s="1"/>
+      <c r="B62" s="65"/>
+      <c r="C62" s="3"/>
+      <c r="D62" s="1"/>
+      <c r="E62" s="4"/>
+      <c r="F62" s="4"/>
+      <c r="G62" s="1"/>
     </row>
     <row r="63">
-      <c r="A63" s="61"/>
-      <c r="B63" s="62"/>
-      <c r="C63" s="63" t="s">
-        <v>82</v>
-      </c>
-      <c r="D63" s="64" t="s">
-        <v>33</v>
-      </c>
-      <c r="E63" s="65"/>
-      <c r="F63" s="65"/>
-      <c r="G63" s="66" t="s">
-        <v>18</v>
-      </c>
+      <c r="A63" s="1"/>
+      <c r="B63" s="65"/>
+      <c r="C63" s="3"/>
+      <c r="D63" s="1"/>
+      <c r="E63" s="4"/>
+      <c r="F63" s="4"/>
+      <c r="G63" s="1"/>
     </row>
     <row r="64">
       <c r="A64" s="1"/>
-      <c r="B64" s="67"/>
+      <c r="B64" s="65"/>
       <c r="C64" s="3"/>
       <c r="D64" s="1"/>
       <c r="E64" s="4"/>
@@ -2031,7 +1975,7 @@
     </row>
     <row r="65">
       <c r="A65" s="1"/>
-      <c r="B65" s="67"/>
+      <c r="B65" s="65"/>
       <c r="C65" s="3"/>
       <c r="D65" s="1"/>
       <c r="E65" s="4"/>
@@ -2040,7 +1984,7 @@
     </row>
     <row r="66">
       <c r="A66" s="1"/>
-      <c r="B66" s="67"/>
+      <c r="B66" s="65"/>
       <c r="C66" s="3"/>
       <c r="D66" s="1"/>
       <c r="E66" s="4"/>
@@ -2049,7 +1993,7 @@
     </row>
     <row r="67">
       <c r="A67" s="1"/>
-      <c r="B67" s="67"/>
+      <c r="B67" s="65"/>
       <c r="C67" s="3"/>
       <c r="D67" s="1"/>
       <c r="E67" s="4"/>
@@ -2058,7 +2002,7 @@
     </row>
     <row r="68">
       <c r="A68" s="1"/>
-      <c r="B68" s="67"/>
+      <c r="B68" s="65"/>
       <c r="C68" s="3"/>
       <c r="D68" s="1"/>
       <c r="E68" s="4"/>
@@ -2067,7 +2011,7 @@
     </row>
     <row r="69">
       <c r="A69" s="1"/>
-      <c r="B69" s="67"/>
+      <c r="B69" s="65"/>
       <c r="C69" s="3"/>
       <c r="D69" s="1"/>
       <c r="E69" s="4"/>
@@ -2076,7 +2020,7 @@
     </row>
     <row r="70">
       <c r="A70" s="1"/>
-      <c r="B70" s="67"/>
+      <c r="B70" s="65"/>
       <c r="C70" s="3"/>
       <c r="D70" s="1"/>
       <c r="E70" s="4"/>
@@ -2085,7 +2029,7 @@
     </row>
     <row r="71">
       <c r="A71" s="1"/>
-      <c r="B71" s="67"/>
+      <c r="B71" s="65"/>
       <c r="C71" s="3"/>
       <c r="D71" s="1"/>
       <c r="E71" s="4"/>
@@ -2094,7 +2038,7 @@
     </row>
     <row r="72">
       <c r="A72" s="1"/>
-      <c r="B72" s="67"/>
+      <c r="B72" s="65"/>
       <c r="C72" s="3"/>
       <c r="D72" s="1"/>
       <c r="E72" s="4"/>
@@ -2103,7 +2047,7 @@
     </row>
     <row r="73">
       <c r="A73" s="1"/>
-      <c r="B73" s="67"/>
+      <c r="B73" s="65"/>
       <c r="C73" s="3"/>
       <c r="D73" s="1"/>
       <c r="E73" s="4"/>
@@ -2112,7 +2056,7 @@
     </row>
     <row r="74">
       <c r="A74" s="1"/>
-      <c r="B74" s="67"/>
+      <c r="B74" s="65"/>
       <c r="C74" s="3"/>
       <c r="D74" s="1"/>
       <c r="E74" s="4"/>
@@ -2121,7 +2065,7 @@
     </row>
     <row r="75">
       <c r="A75" s="1"/>
-      <c r="B75" s="67"/>
+      <c r="B75" s="65"/>
       <c r="C75" s="3"/>
       <c r="D75" s="1"/>
       <c r="E75" s="4"/>
@@ -2130,7 +2074,7 @@
     </row>
     <row r="76">
       <c r="A76" s="1"/>
-      <c r="B76" s="67"/>
+      <c r="B76" s="65"/>
       <c r="C76" s="3"/>
       <c r="D76" s="1"/>
       <c r="E76" s="4"/>
@@ -2139,7 +2083,7 @@
     </row>
     <row r="77">
       <c r="A77" s="1"/>
-      <c r="B77" s="67"/>
+      <c r="B77" s="65"/>
       <c r="C77" s="3"/>
       <c r="D77" s="1"/>
       <c r="E77" s="4"/>
@@ -2148,7 +2092,7 @@
     </row>
     <row r="78">
       <c r="A78" s="1"/>
-      <c r="B78" s="67"/>
+      <c r="B78" s="65"/>
       <c r="C78" s="3"/>
       <c r="D78" s="1"/>
       <c r="E78" s="4"/>
@@ -2157,7 +2101,7 @@
     </row>
     <row r="79">
       <c r="A79" s="1"/>
-      <c r="B79" s="67"/>
+      <c r="B79" s="65"/>
       <c r="C79" s="3"/>
       <c r="D79" s="1"/>
       <c r="E79" s="4"/>
@@ -2166,7 +2110,7 @@
     </row>
     <row r="80">
       <c r="A80" s="1"/>
-      <c r="B80" s="67"/>
+      <c r="B80" s="65"/>
       <c r="C80" s="3"/>
       <c r="D80" s="1"/>
       <c r="E80" s="4"/>
@@ -2175,7 +2119,7 @@
     </row>
     <row r="81">
       <c r="A81" s="1"/>
-      <c r="B81" s="67"/>
+      <c r="B81" s="65"/>
       <c r="C81" s="3"/>
       <c r="D81" s="1"/>
       <c r="E81" s="4"/>
@@ -2184,7 +2128,7 @@
     </row>
     <row r="82">
       <c r="A82" s="1"/>
-      <c r="B82" s="67"/>
+      <c r="B82" s="65"/>
       <c r="C82" s="3"/>
       <c r="D82" s="1"/>
       <c r="E82" s="4"/>
@@ -2193,7 +2137,7 @@
     </row>
     <row r="83">
       <c r="A83" s="1"/>
-      <c r="B83" s="67"/>
+      <c r="B83" s="65"/>
       <c r="C83" s="3"/>
       <c r="D83" s="1"/>
       <c r="E83" s="4"/>
@@ -2202,7 +2146,7 @@
     </row>
     <row r="84">
       <c r="A84" s="1"/>
-      <c r="B84" s="67"/>
+      <c r="B84" s="65"/>
       <c r="C84" s="3"/>
       <c r="D84" s="1"/>
       <c r="E84" s="4"/>
@@ -2211,7 +2155,7 @@
     </row>
     <row r="85">
       <c r="A85" s="1"/>
-      <c r="B85" s="67"/>
+      <c r="B85" s="65"/>
       <c r="C85" s="3"/>
       <c r="D85" s="1"/>
       <c r="E85" s="4"/>
@@ -2220,7 +2164,7 @@
     </row>
     <row r="86">
       <c r="A86" s="1"/>
-      <c r="B86" s="67"/>
+      <c r="B86" s="65"/>
       <c r="C86" s="3"/>
       <c r="D86" s="1"/>
       <c r="E86" s="4"/>
@@ -2229,7 +2173,7 @@
     </row>
     <row r="87">
       <c r="A87" s="1"/>
-      <c r="B87" s="67"/>
+      <c r="B87" s="65"/>
       <c r="C87" s="3"/>
       <c r="D87" s="1"/>
       <c r="E87" s="4"/>
@@ -2238,7 +2182,7 @@
     </row>
     <row r="88">
       <c r="A88" s="1"/>
-      <c r="B88" s="67"/>
+      <c r="B88" s="65"/>
       <c r="C88" s="3"/>
       <c r="D88" s="1"/>
       <c r="E88" s="4"/>
@@ -2247,7 +2191,7 @@
     </row>
     <row r="89">
       <c r="A89" s="1"/>
-      <c r="B89" s="67"/>
+      <c r="B89" s="65"/>
       <c r="C89" s="3"/>
       <c r="D89" s="1"/>
       <c r="E89" s="4"/>
@@ -2256,7 +2200,7 @@
     </row>
     <row r="90">
       <c r="A90" s="1"/>
-      <c r="B90" s="67"/>
+      <c r="B90" s="65"/>
       <c r="C90" s="3"/>
       <c r="D90" s="1"/>
       <c r="E90" s="4"/>
@@ -2265,7 +2209,7 @@
     </row>
     <row r="91">
       <c r="A91" s="1"/>
-      <c r="B91" s="67"/>
+      <c r="B91" s="65"/>
       <c r="C91" s="3"/>
       <c r="D91" s="1"/>
       <c r="E91" s="4"/>
@@ -2274,7 +2218,7 @@
     </row>
     <row r="92">
       <c r="A92" s="1"/>
-      <c r="B92" s="67"/>
+      <c r="B92" s="65"/>
       <c r="C92" s="3"/>
       <c r="D92" s="1"/>
       <c r="E92" s="4"/>
@@ -2283,7 +2227,7 @@
     </row>
     <row r="93">
       <c r="A93" s="1"/>
-      <c r="B93" s="67"/>
+      <c r="B93" s="65"/>
       <c r="C93" s="3"/>
       <c r="D93" s="1"/>
       <c r="E93" s="4"/>
@@ -2292,7 +2236,7 @@
     </row>
     <row r="94">
       <c r="A94" s="1"/>
-      <c r="B94" s="67"/>
+      <c r="B94" s="65"/>
       <c r="C94" s="3"/>
       <c r="D94" s="1"/>
       <c r="E94" s="4"/>
@@ -2301,7 +2245,7 @@
     </row>
     <row r="95">
       <c r="A95" s="1"/>
-      <c r="B95" s="67"/>
+      <c r="B95" s="65"/>
       <c r="C95" s="3"/>
       <c r="D95" s="1"/>
       <c r="E95" s="4"/>
@@ -2310,7 +2254,7 @@
     </row>
     <row r="96">
       <c r="A96" s="1"/>
-      <c r="B96" s="67"/>
+      <c r="B96" s="65"/>
       <c r="C96" s="3"/>
       <c r="D96" s="1"/>
       <c r="E96" s="4"/>
@@ -2319,7 +2263,7 @@
     </row>
     <row r="97">
       <c r="A97" s="1"/>
-      <c r="B97" s="67"/>
+      <c r="B97" s="65"/>
       <c r="C97" s="3"/>
       <c r="D97" s="1"/>
       <c r="E97" s="4"/>
@@ -2328,7 +2272,7 @@
     </row>
     <row r="98">
       <c r="A98" s="1"/>
-      <c r="B98" s="67"/>
+      <c r="B98" s="65"/>
       <c r="C98" s="3"/>
       <c r="D98" s="1"/>
       <c r="E98" s="4"/>
@@ -2337,7 +2281,7 @@
     </row>
     <row r="99">
       <c r="A99" s="1"/>
-      <c r="B99" s="67"/>
+      <c r="B99" s="65"/>
       <c r="C99" s="3"/>
       <c r="D99" s="1"/>
       <c r="E99" s="4"/>
@@ -2346,7 +2290,7 @@
     </row>
     <row r="100">
       <c r="A100" s="1"/>
-      <c r="B100" s="67"/>
+      <c r="B100" s="65"/>
       <c r="C100" s="3"/>
       <c r="D100" s="1"/>
       <c r="E100" s="4"/>
@@ -2355,7 +2299,7 @@
     </row>
     <row r="101">
       <c r="A101" s="1"/>
-      <c r="B101" s="67"/>
+      <c r="B101" s="65"/>
       <c r="C101" s="3"/>
       <c r="D101" s="1"/>
       <c r="E101" s="4"/>
@@ -2364,7 +2308,7 @@
     </row>
     <row r="102">
       <c r="A102" s="1"/>
-      <c r="B102" s="67"/>
+      <c r="B102" s="65"/>
       <c r="C102" s="3"/>
       <c r="D102" s="1"/>
       <c r="E102" s="4"/>
@@ -2373,7 +2317,7 @@
     </row>
     <row r="103">
       <c r="A103" s="1"/>
-      <c r="B103" s="67"/>
+      <c r="B103" s="65"/>
       <c r="C103" s="3"/>
       <c r="D103" s="1"/>
       <c r="E103" s="4"/>
@@ -2382,7 +2326,7 @@
     </row>
     <row r="104">
       <c r="A104" s="1"/>
-      <c r="B104" s="67"/>
+      <c r="B104" s="65"/>
       <c r="C104" s="3"/>
       <c r="D104" s="1"/>
       <c r="E104" s="4"/>
@@ -2391,7 +2335,7 @@
     </row>
     <row r="105">
       <c r="A105" s="1"/>
-      <c r="B105" s="67"/>
+      <c r="B105" s="65"/>
       <c r="C105" s="3"/>
       <c r="D105" s="1"/>
       <c r="E105" s="4"/>
@@ -2400,7 +2344,7 @@
     </row>
     <row r="106">
       <c r="A106" s="1"/>
-      <c r="B106" s="67"/>
+      <c r="B106" s="65"/>
       <c r="C106" s="3"/>
       <c r="D106" s="1"/>
       <c r="E106" s="4"/>
@@ -2409,7 +2353,7 @@
     </row>
     <row r="107">
       <c r="A107" s="1"/>
-      <c r="B107" s="67"/>
+      <c r="B107" s="65"/>
       <c r="C107" s="3"/>
       <c r="D107" s="1"/>
       <c r="E107" s="4"/>
@@ -2418,7 +2362,7 @@
     </row>
     <row r="108">
       <c r="A108" s="1"/>
-      <c r="B108" s="67"/>
+      <c r="B108" s="65"/>
       <c r="C108" s="3"/>
       <c r="D108" s="1"/>
       <c r="E108" s="4"/>
@@ -2427,7 +2371,7 @@
     </row>
     <row r="109">
       <c r="A109" s="1"/>
-      <c r="B109" s="67"/>
+      <c r="B109" s="2"/>
       <c r="C109" s="3"/>
       <c r="D109" s="1"/>
       <c r="E109" s="4"/>
@@ -2436,7 +2380,7 @@
     </row>
     <row r="110">
       <c r="A110" s="1"/>
-      <c r="B110" s="67"/>
+      <c r="B110" s="2"/>
       <c r="C110" s="3"/>
       <c r="D110" s="1"/>
       <c r="E110" s="4"/>
@@ -2445,7 +2389,7 @@
     </row>
     <row r="111">
       <c r="A111" s="1"/>
-      <c r="B111" s="67"/>
+      <c r="B111" s="2"/>
       <c r="C111" s="3"/>
       <c r="D111" s="1"/>
       <c r="E111" s="4"/>
@@ -2454,7 +2398,7 @@
     </row>
     <row r="112">
       <c r="A112" s="1"/>
-      <c r="B112" s="67"/>
+      <c r="B112" s="2"/>
       <c r="C112" s="3"/>
       <c r="D112" s="1"/>
       <c r="E112" s="4"/>
@@ -2463,7 +2407,7 @@
     </row>
     <row r="113">
       <c r="A113" s="1"/>
-      <c r="B113" s="67"/>
+      <c r="B113" s="2"/>
       <c r="C113" s="3"/>
       <c r="D113" s="1"/>
       <c r="E113" s="4"/>
@@ -2472,7 +2416,7 @@
     </row>
     <row r="114">
       <c r="A114" s="1"/>
-      <c r="B114" s="67"/>
+      <c r="B114" s="2"/>
       <c r="C114" s="3"/>
       <c r="D114" s="1"/>
       <c r="E114" s="4"/>
@@ -10354,62 +10298,8 @@
       <c r="F989" s="4"/>
       <c r="G989" s="1"/>
     </row>
-    <row r="990">
-      <c r="A990" s="1"/>
-      <c r="B990" s="2"/>
-      <c r="C990" s="3"/>
-      <c r="D990" s="1"/>
-      <c r="E990" s="4"/>
-      <c r="F990" s="4"/>
-      <c r="G990" s="1"/>
-    </row>
-    <row r="991">
-      <c r="A991" s="1"/>
-      <c r="B991" s="2"/>
-      <c r="C991" s="3"/>
-      <c r="D991" s="1"/>
-      <c r="E991" s="4"/>
-      <c r="F991" s="4"/>
-      <c r="G991" s="1"/>
-    </row>
-    <row r="992">
-      <c r="A992" s="1"/>
-      <c r="B992" s="2"/>
-      <c r="C992" s="3"/>
-      <c r="D992" s="1"/>
-      <c r="E992" s="4"/>
-      <c r="F992" s="4"/>
-      <c r="G992" s="1"/>
-    </row>
-    <row r="993">
-      <c r="A993" s="1"/>
-      <c r="B993" s="2"/>
-      <c r="C993" s="3"/>
-      <c r="D993" s="1"/>
-      <c r="E993" s="4"/>
-      <c r="F993" s="4"/>
-      <c r="G993" s="1"/>
-    </row>
-    <row r="994">
-      <c r="A994" s="1"/>
-      <c r="B994" s="2"/>
-      <c r="C994" s="3"/>
-      <c r="D994" s="1"/>
-      <c r="E994" s="4"/>
-      <c r="F994" s="4"/>
-      <c r="G994" s="1"/>
-    </row>
-    <row r="995">
-      <c r="A995" s="1"/>
-      <c r="B995" s="2"/>
-      <c r="C995" s="3"/>
-      <c r="D995" s="1"/>
-      <c r="E995" s="4"/>
-      <c r="F995" s="4"/>
-      <c r="G995" s="1"/>
-    </row>
   </sheetData>
-  <mergeCells count="23">
+  <mergeCells count="21">
     <mergeCell ref="A2:G2"/>
     <mergeCell ref="A4:A6"/>
     <mergeCell ref="B4:B6"/>
@@ -10417,29 +10307,27 @@
     <mergeCell ref="B7:B12"/>
     <mergeCell ref="A13:A19"/>
     <mergeCell ref="B13:B19"/>
-    <mergeCell ref="A38:A42"/>
-    <mergeCell ref="A43:A47"/>
-    <mergeCell ref="A48:A54"/>
-    <mergeCell ref="A55:A57"/>
-    <mergeCell ref="A58:A63"/>
-    <mergeCell ref="B43:B47"/>
-    <mergeCell ref="B48:B54"/>
-    <mergeCell ref="B55:B57"/>
-    <mergeCell ref="B58:B63"/>
-    <mergeCell ref="A20:A26"/>
-    <mergeCell ref="B20:B26"/>
-    <mergeCell ref="A27:A33"/>
-    <mergeCell ref="B27:B33"/>
-    <mergeCell ref="A34:A37"/>
-    <mergeCell ref="B34:B37"/>
-    <mergeCell ref="B38:B42"/>
+    <mergeCell ref="A32:A36"/>
+    <mergeCell ref="A37:A41"/>
+    <mergeCell ref="A42:A48"/>
+    <mergeCell ref="A49:A51"/>
+    <mergeCell ref="A52:A57"/>
+    <mergeCell ref="B37:B41"/>
+    <mergeCell ref="B42:B48"/>
+    <mergeCell ref="B49:B51"/>
+    <mergeCell ref="B52:B57"/>
+    <mergeCell ref="A20:A27"/>
+    <mergeCell ref="B20:B27"/>
+    <mergeCell ref="A28:A31"/>
+    <mergeCell ref="B28:B31"/>
+    <mergeCell ref="B32:B36"/>
   </mergeCells>
-  <conditionalFormatting sqref="E1 E3:E995">
+  <conditionalFormatting sqref="E1 E3:E989">
     <cfRule type="notContainsBlanks" dxfId="0" priority="1">
       <formula>LEN(TRIM(E1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F1 F3:F995">
+  <conditionalFormatting sqref="F1 F3:F989">
     <cfRule type="notContainsBlanks" dxfId="1" priority="2">
       <formula>LEN(TRIM(F1))&gt;0</formula>
     </cfRule>

</xml_diff>